<commit_message>
added past data for comparison
</commit_message>
<xml_diff>
--- a/Education/enrollment/mean-years-of-schooling-by-sex-annual (1980-2018).xlsx
+++ b/Education/enrollment/mean-years-of-schooling-by-sex-annual (1980-2018).xlsx
@@ -5,42 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\mean-years-of-schooling-annual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\github stuff\BAVP\Education\enrollment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3ABFDE6-4629-42EA-AEFA-7894819EC2AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FBF4A15-BE6C-41C6-8241-842EA367EF57}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9818" yWindow="-15458" windowWidth="19395" windowHeight="14955"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395"/>
   </bookViews>
   <sheets>
-    <sheet name="mean-years-of-schooling-by-sex-" sheetId="1" r:id="rId1"/>
+    <sheet name="Output" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>level_1</t>
-  </si>
-  <si>
-    <t>level_2</t>
+    <t>gender</t>
   </si>
   <si>
     <t>value</t>
   </si>
   <si>
-    <t>Mean Years Of Schooling (25 Years &amp; Over)</t>
+    <t>M</t>
   </si>
   <si>
-    <t>Males</t>
-  </si>
-  <si>
-    <t>Females</t>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -881,13 +875,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -897,1043 +891,818 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1980</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>5.6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1980</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>3.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1983</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>6.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1983</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1984</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>6.6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1984</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
+      <c r="C7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1985</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="C8">
         <v>6.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1985</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1986</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="C10">
         <v>6.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1986</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1987</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="C12">
         <v>6.6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1987</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
         <v>5.2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1988</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="C14">
         <v>6.9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1988</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
+      <c r="C15">
         <v>5.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1989</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="C16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1989</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
+      <c r="C17">
         <v>5.6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1990</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="C18">
         <v>7.3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1990</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
         <v>5.9</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1991</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="C20">
         <v>7.6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1991</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
+      <c r="C21">
         <v>6.2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1992</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="C22">
         <v>7.8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>1992</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
+      <c r="C23">
         <v>6.3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>1993</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="C24">
         <v>7.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>1993</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
+      <c r="C25">
         <v>6.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1994</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="C26">
         <v>8.1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>1994</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
         <v>6.6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>1995</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="C28">
         <v>8.4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>1995</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
         <v>7.2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>1996</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="C30">
         <v>8.4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>1996</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
+      <c r="C31">
         <v>7.1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>1997</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="C32">
         <v>8.6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>1997</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33">
+      <c r="C33">
         <v>7.2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>1998</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="C34">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>1998</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35">
+      <c r="C35">
         <v>7.4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>1999</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="C36">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>1999</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37">
+      <c r="C37">
         <v>7.6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>2000</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="C38">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>2000</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
+      <c r="C39">
         <v>8.1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>2001</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="C40">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>2001</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
+      <c r="C41">
         <v>7.9</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>2002</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="C42">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>2002</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43">
+      <c r="C43">
         <v>8.1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>2003</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="C44">
         <v>9.4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>2003</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45">
+      <c r="C45">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>2004</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="C46">
         <v>9.6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>2004</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47">
+      <c r="C47">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>2005</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="C48">
         <v>9.9</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>2005</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49">
+      <c r="C49">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>2006</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="C50">
         <v>9.9</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>2006</v>
       </c>
       <c r="B51" t="s">
         <v>4</v>
       </c>
-      <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51">
+      <c r="C51">
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>2007</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="C52">
         <v>9.9</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>2007</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
       </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53">
+      <c r="C53">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>2008</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="C54">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>2008</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
       </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55">
+      <c r="C55">
         <v>9.1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>2009</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="C56">
         <v>10.3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>2009</v>
       </c>
       <c r="B57" t="s">
         <v>4</v>
       </c>
-      <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57">
+      <c r="C57">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>2010</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="C58">
         <v>10.6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>2010</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
       </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59">
+      <c r="C59">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>2011</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="C60">
         <v>10.7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>2011</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
       </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61">
+      <c r="C61">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>2012</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="C62">
         <v>10.9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>2012</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
       </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63">
+      <c r="C63">
         <v>9.9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>2013</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="C64">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>2013</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
-      <c r="C65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65">
+      <c r="C65">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>2014</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="C66">
         <v>11.1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>2014</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67">
+      <c r="C67">
         <v>10.1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>2015</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="C68">
         <v>11.2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>2015</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69">
+      <c r="C69">
         <v>10.3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>2016</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
-      </c>
-      <c r="C70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="C70">
         <v>11.2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>2016</v>
       </c>
       <c r="B71" t="s">
         <v>4</v>
       </c>
-      <c r="C71" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71">
+      <c r="C71">
         <v>10.3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>2017</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="C72">
         <v>11.3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>2017</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
       </c>
-      <c r="C73" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73">
+      <c r="C73">
         <v>10.4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>2018</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="C74">
         <v>11.6</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>2018</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
       </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75">
+      <c r="C75">
         <v>10.6</v>
       </c>
     </row>

</xml_diff>